<commit_message>
Final version of RASD, DD, Code inspection and Testing
</commit_message>
<xml_diff>
--- a/Deliverables/RASD/Use Case specification 0.2.xlsx
+++ b/Deliverables/RASD/Use Case specification 0.2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="645" windowWidth="16590" windowHeight="8415"/>
+    <workbookView xWindow="4395" yWindow="645" windowWidth="16590" windowHeight="8415" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="UC-01" sheetId="18" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="114">
   <si>
     <t>No.</t>
   </si>
@@ -212,40 +212,11 @@
     <t>Informs the system that he accepts the request.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Sends the </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>incoming request information</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to the first available taxi driver in the zone's queue.</t>
-    </r>
-  </si>
-  <si>
     <t>Change the status of the taxi driver to not available.</t>
   </si>
   <si>
     <t>The taxi driver has accepted the request.
 The passenger is waiting for the system to reply to his request.</t>
-  </si>
-  <si>
-    <t>6.1. The zone's queue is empty or every taxi driver cancels the request:
-- The system informs the passenger(s) that it is impossible to find a taxi driver.
-- The Use Case ends.</t>
   </si>
   <si>
     <t>7.1. The taxi driver does not accept the request:
@@ -275,9 +246,6 @@
   </si>
   <si>
     <t>Confirms to the passenger that his cancel request has been taking to account.</t>
-  </si>
-  <si>
-    <t>Sends a message to the concerning taxi driver to inform him that the ride has been cancelled</t>
   </si>
   <si>
     <t>Puts the taxi driver at the top of the queue of the area he is related now</t>
@@ -685,9 +653,83 @@
     <t>Creates the passenger account in the MyTaxiService system.</t>
   </si>
   <si>
+    <t>3.1. The received information is not correct or complete:
+- The system informs the passeger that the sent information is wrong or incomplete.
+- Return to step 1.</t>
+  </si>
+  <si>
+    <t>The passenger is logged in MyTaxiService.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sends a form to the passengr with fields already filled corresponding to his personal information and two fields </t>
+  </si>
+  <si>
+    <t>6.1. The received information is not correct or complete:
+- The system informs the passeger that the sent information is wrong or incomplete.
+- Return to step 1.</t>
+  </si>
+  <si>
+    <t>Asks the passenger his email address and password.</t>
+  </si>
+  <si>
+    <t>Replies the system with his email address and password.</t>
+  </si>
+  <si>
+    <t>3.1 The passenger select: "Changes my password" :
+- The system send a three forms field, two for the same new password, one for the current one
+- The passeger fills the form
+- Return to the step 5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sends the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>incoming request information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to the first available taxi driver in the zone's queue whose capacity is greater or equal than the amount of people.</t>
+    </r>
+  </si>
+  <si>
+    <t>6.1. The zone queue is empty:
+- The system tries to find taxi drivers in the closest adjacent zones to the origins of the request (or the origin of thr first request for sharing requests)
+- Return to step 6.</t>
+  </si>
+  <si>
+    <t>Sends a message to the concerning taxi driver and passenger(s) to inform him that the ride has been cancelled</t>
+  </si>
+  <si>
+    <t>6.1. No accepting taxi driver is found within three minutes (neither in the one nor in the adjacent ones):
+- The system informs the passenger(s) that it is impossible to find a taxi driver.
+- The Use Case ends.</t>
+  </si>
+  <si>
+    <t>7.2. The taxi driver does not respond in less than 30 seconds:
+- The system sends the taxi driver to the bottom of the zone's queue.
+- Return to step 6.</t>
+  </si>
+  <si>
+    <t>Sends confirmation email to the passenger</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">The passenger is already registered in MyTaxiService.
-The taxi driver has not logged in MyTaxiService yet.
+The passeger has already confirmed his email address.
+The passenger has not logged in MyTaxiService yet.
 The passenger has launched the MyTaxiService mobile application or is the website.
 The passenger selects the option </t>
     </r>
@@ -710,17 +752,6 @@
       </rPr>
       <t>.</t>
     </r>
-  </si>
-  <si>
-    <t>3.1. The received information is not correct or complete:
-- The system informs the passeger that the sent information is wrong or incomplete.
-- Return to step 1.</t>
-  </si>
-  <si>
-    <t>3.1 The passenger select: "Changes my password" :
-- The system send a three forms field, two for the same new password, one for the current one
-- The taxi drivers fills the form
-- Return to the step 5</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1035,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1673,12 +1704,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF333399"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF333399"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF333399"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF333399"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF333399"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF333399"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF333399"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF333399"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF333399"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1797,29 +1867,88 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1836,76 +1965,136 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1914,35 +2103,69 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1953,63 +2176,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2035,27 +2221,6 @@
     <xf numFmtId="0" fontId="21" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2065,93 +2230,19 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2465,9 +2556,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I30"/>
+  <dimension ref="B1:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2502,10 +2593,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -2535,73 +2626,73 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
     <row r="7" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
     </row>
     <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="172" t="s">
+      <c r="B9" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="173"/>
-      <c r="D9" s="169" t="s">
+      <c r="C9" s="63"/>
+      <c r="D9" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="170"/>
-      <c r="F9" s="171"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66"/>
       <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:9" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="75" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75"/>
       <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2613,108 +2704,112 @@
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="52"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="79"/>
       <c r="H13" s="30"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="59" t="s">
+      <c r="C14" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="83"/>
+      <c r="E14" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="61"/>
+      <c r="F14" s="84"/>
     </row>
     <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="58"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
     </row>
     <row r="16" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="34">
         <v>1</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="70" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="175"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="87"/>
     </row>
     <row r="17" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="33">
         <v>2</v>
       </c>
-      <c r="C17" s="70" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="174"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="64"/>
+      <c r="C17" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="90"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="91"/>
     </row>
     <row r="18" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="33">
         <v>3</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="70" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="175"/>
-    </row>
-    <row r="19" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="32">
+      <c r="C18" s="85"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="87"/>
+    </row>
+    <row r="19" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="33">
         <v>4</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="49"/>
-    </row>
-    <row r="20" spans="2:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="31"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-    </row>
-    <row r="21" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
+      <c r="C19" s="181"/>
+      <c r="D19" s="182"/>
+      <c r="E19" s="183" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="184"/>
+    </row>
+    <row r="20" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="32">
+        <v>5</v>
+      </c>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="89"/>
+    </row>
+    <row r="21" spans="2:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="31"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
-    <row r="22" spans="2:6" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="53" t="s">
+    <row r="22" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="78"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+    </row>
+    <row r="23" spans="2:6" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-    </row>
-    <row r="23" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="75"/>
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
     </row>
@@ -2767,21 +2862,16 @@
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
     </row>
+    <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B22:D22"/>
+  <mergeCells count="28">
+    <mergeCell ref="B23:D23"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:D15"/>
@@ -2790,11 +2880,25 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B22:D22"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2803,7 +2907,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I28"/>
+  <dimension ref="B1:I29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -2840,10 +2944,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -2873,164 +2977,169 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
     <row r="7" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
     </row>
     <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
     </row>
-    <row r="9" spans="2:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="92" t="s">
+    <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="63"/>
+      <c r="D9" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66"/>
+      <c r="H9" s="30"/>
+    </row>
+    <row r="10" spans="2:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="97"/>
-      <c r="D9" s="98" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="99"/>
-      <c r="F9" s="100"/>
-      <c r="H9" s="30"/>
-    </row>
-    <row r="10" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="101" t="s">
+      <c r="C10" s="100"/>
+      <c r="D10" s="101" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="102"/>
+      <c r="F10" s="103"/>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="103" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="104"/>
-      <c r="F10" s="105"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="106" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
       <c r="H11" s="30"/>
     </row>
-    <row r="12" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="84" t="s">
+    <row r="12" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="H12" s="30"/>
+    </row>
+    <row r="13" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85"/>
-      <c r="F12" s="86"/>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="87" t="s">
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="95"/>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="89" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="90"/>
-      <c r="E13" s="89" t="s">
+      <c r="C14" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="114"/>
+      <c r="E14" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="91"/>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="88"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="91"/>
-    </row>
-    <row r="15" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="14">
+      <c r="F14" s="115"/>
+      <c r="H14" s="30"/>
+    </row>
+    <row r="15" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="112"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="115"/>
+    </row>
+    <row r="16" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="14">
         <v>1</v>
       </c>
-      <c r="C15" s="81"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="81" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="83"/>
-    </row>
-    <row r="16" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="21">
+      <c r="C16" s="107"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="107" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" s="109"/>
+    </row>
+    <row r="17" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="21">
         <v>2</v>
       </c>
-      <c r="C16" s="81" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="82"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="83"/>
-    </row>
-    <row r="17" spans="2:6" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="32">
+      <c r="C17" s="107" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="108"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="109"/>
+    </row>
+    <row r="18" spans="2:6" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="32">
         <v>3</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="49"/>
-    </row>
-    <row r="18" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="31"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-    </row>
-    <row r="19" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="112" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="85"/>
-      <c r="D19" s="86"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="89"/>
+    </row>
+    <row r="19" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="31"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
     </row>
-    <row r="20" spans="2:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="106" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="104"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-    </row>
-    <row r="21" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
+    <row r="20" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="94"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="2:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="96" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="97"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
     </row>
@@ -3083,30 +3192,39 @@
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
     </row>
+    <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+    </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
+  <mergeCells count="24">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3115,7 +3233,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I30"/>
+  <dimension ref="B1:I31"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3134,7 +3252,7 @@
     <row r="1" spans="2:9" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="45" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="43"/>
@@ -3152,10 +3270,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -3185,226 +3303,232 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
     <row r="7" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
     </row>
     <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="172" t="s">
+      <c r="B9" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="173"/>
-      <c r="D9" s="169" t="s">
+      <c r="C9" s="63"/>
+      <c r="D9" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="170"/>
-      <c r="F9" s="171"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66"/>
       <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="148"/>
-      <c r="D10" s="150" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="150"/>
-      <c r="F10" s="150"/>
+      <c r="C10" s="121"/>
+      <c r="D10" s="122" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="151" t="s">
+      <c r="B11" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="151"/>
-      <c r="D11" s="152" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="152"/>
-      <c r="F11" s="152"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="124" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
       <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="153"/>
-      <c r="C12" s="154"/>
-      <c r="D12" s="154"/>
-      <c r="E12" s="154"/>
-      <c r="F12" s="154"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="155"/>
-      <c r="E13" s="155"/>
-      <c r="F13" s="155"/>
+      <c r="C13" s="125"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="125"/>
       <c r="H13" s="30"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="157" t="s">
+      <c r="C14" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="157"/>
-      <c r="E14" s="158" t="s">
+      <c r="D14" s="127"/>
+      <c r="E14" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="158"/>
+      <c r="F14" s="128"/>
     </row>
     <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="156"/>
-      <c r="C15" s="157"/>
-      <c r="D15" s="157"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="127"/>
+      <c r="D15" s="127"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="128"/>
     </row>
     <row r="16" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="159">
+      <c r="B16" s="50">
         <v>1</v>
       </c>
-      <c r="C16" s="177" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16" s="177"/>
-      <c r="E16" s="178"/>
-      <c r="F16" s="178"/>
+      <c r="C16" s="129" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="129"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="130"/>
     </row>
     <row r="17" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="159">
+      <c r="B17" s="50">
         <v>2</v>
       </c>
-      <c r="C17" s="177" t="s">
+      <c r="C17" s="129" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="129"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="130"/>
+    </row>
+    <row r="18" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="51">
+        <v>3</v>
+      </c>
+      <c r="C18" s="129" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="129"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="130"/>
+    </row>
+    <row r="19" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="51">
+        <v>4</v>
+      </c>
+      <c r="C19" s="129"/>
+      <c r="D19" s="129"/>
+      <c r="E19" s="130" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="130"/>
+    </row>
+    <row r="20" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="51">
+        <v>5</v>
+      </c>
+      <c r="C20" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="177"/>
-      <c r="E17" s="178"/>
-      <c r="F17" s="178"/>
-    </row>
-    <row r="18" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="162">
-        <v>3</v>
-      </c>
-      <c r="C18" s="177" t="s">
+      <c r="D20" s="129"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="130"/>
+    </row>
+    <row r="21" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="51">
+        <v>6</v>
+      </c>
+      <c r="C21" s="129"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="131" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="177"/>
-      <c r="E18" s="178"/>
-      <c r="F18" s="178"/>
-    </row>
-    <row r="19" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="162">
-        <v>4</v>
-      </c>
-      <c r="C19" s="177"/>
-      <c r="D19" s="177"/>
-      <c r="E19" s="178" t="s">
+      <c r="F21" s="132"/>
+    </row>
+    <row r="22" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="51">
+        <v>7</v>
+      </c>
+      <c r="C22" s="131"/>
+      <c r="D22" s="185"/>
+      <c r="E22" s="183" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="184"/>
+    </row>
+    <row r="23" spans="2:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="52">
+        <v>8</v>
+      </c>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="178"/>
-    </row>
-    <row r="20" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="162">
-        <v>5</v>
-      </c>
-      <c r="C20" s="177" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="177"/>
-      <c r="E20" s="178"/>
-      <c r="F20" s="178"/>
-    </row>
-    <row r="21" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="162">
-        <v>6</v>
-      </c>
-      <c r="C21" s="177" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="177"/>
-      <c r="E21" s="178"/>
-      <c r="F21" s="178"/>
-    </row>
-    <row r="22" spans="2:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="163">
-        <v>7</v>
-      </c>
-      <c r="C22" s="164"/>
-      <c r="D22" s="164"/>
-      <c r="E22" s="165" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="165"/>
-    </row>
-    <row r="23" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="153"/>
-      <c r="C23" s="154"/>
-      <c r="D23" s="154"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-    </row>
-    <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="166" t="s">
+      <c r="F23" s="118"/>
+    </row>
+    <row r="24" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="48"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+    </row>
+    <row r="25" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="166"/>
-      <c r="D24" s="166"/>
-      <c r="E24" s="154"/>
-      <c r="F24" s="154"/>
-    </row>
-    <row r="25" spans="2:6" ht="78" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="176" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" s="167"/>
-      <c r="D25" s="167"/>
-      <c r="E25" s="168"/>
-      <c r="F25" s="168"/>
-    </row>
-    <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-    </row>
-    <row r="27" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+    </row>
+    <row r="26" spans="2:6" ht="78" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="119" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="120"/>
+      <c r="D26" s="120"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+    </row>
+    <row r="27" spans="2:6" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="96" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="97"/>
+      <c r="D27" s="98"/>
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
     </row>
@@ -3429,40 +3553,50 @@
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
     </row>
+    <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+    </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="B24:D24"/>
+  <mergeCells count="35">
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3490,7 +3624,7 @@
     <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="43"/>
@@ -3508,10 +3642,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -3539,68 +3673,68 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="G6" s="30"/>
     </row>
     <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="G7" s="30"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="67" t="s">
+      <c r="C9" s="133"/>
+      <c r="D9" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="68"/>
-      <c r="F9" s="69"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="61"/>
     </row>
     <row r="10" spans="2:7" s="35" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="75" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
     </row>
     <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="31"/>
@@ -3610,77 +3744,77 @@
       <c r="F12" s="30"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="52"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="79"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="59" t="s">
+      <c r="D14" s="83"/>
+      <c r="E14" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="61"/>
+      <c r="F14" s="84"/>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="58"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
     </row>
     <row r="16" spans="2:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="34">
         <v>1</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="64"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="85" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="91"/>
     </row>
     <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="33">
         <v>2</v>
       </c>
-      <c r="C17" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="64"/>
+      <c r="C17" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="86"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="91"/>
     </row>
     <row r="18" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="33">
         <v>3</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="64"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="91"/>
     </row>
     <row r="19" spans="2:6" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="32">
         <v>4</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="49"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="89"/>
     </row>
     <row r="20" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="31"/>
@@ -3690,20 +3824,20 @@
       <c r="F20" s="30"/>
     </row>
     <row r="21" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="79"/>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
     <row r="22" spans="2:6" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
+      <c r="B22" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="74"/>
+      <c r="D22" s="75"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
     </row>
@@ -3751,6 +3885,18 @@
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B13:F13"/>
@@ -3765,18 +3911,6 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3804,7 +3938,7 @@
     <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="45" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="43"/>
@@ -3822,10 +3956,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -3853,68 +3987,68 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="G6" s="30"/>
     </row>
     <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="G7" s="30"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="93"/>
-      <c r="D9" s="94" t="s">
+      <c r="C9" s="134"/>
+      <c r="D9" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="95"/>
-      <c r="F9" s="96"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="137"/>
     </row>
     <row r="10" spans="2:7" s="35" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="98" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="99"/>
-      <c r="F10" s="100"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="102"/>
+      <c r="F10" s="103"/>
     </row>
     <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="103" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="104"/>
-      <c r="F11" s="105"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="106" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
@@ -3924,66 +4058,66 @@
       <c r="F12" s="17"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="86"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="95"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="90"/>
-      <c r="E14" s="89" t="s">
+      <c r="D14" s="114"/>
+      <c r="E14" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="91"/>
+      <c r="F14" s="115"/>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="88"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="91"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="115"/>
     </row>
     <row r="16" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="14">
         <v>1</v>
       </c>
-      <c r="C16" s="81"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="81" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="83"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="107" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="109"/>
     </row>
     <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21">
         <v>2</v>
       </c>
-      <c r="C17" s="81" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="82"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="83"/>
+      <c r="C17" s="107" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="108"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="109"/>
     </row>
     <row r="18" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="32">
         <v>3</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="49"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="89"/>
     </row>
     <row r="19" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="31"/>
@@ -3993,20 +4127,20 @@
       <c r="F19" s="30"/>
     </row>
     <row r="20" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="112" t="s">
+      <c r="B20" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="85"/>
-      <c r="D20" s="86"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="95"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
     </row>
     <row r="21" spans="2:6" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="106" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="104"/>
-      <c r="D21" s="105"/>
+      <c r="B21" s="96" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="97"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
     </row>
@@ -4054,18 +4188,6 @@
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="C17:D17"/>
@@ -4078,6 +4200,18 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4105,7 +4239,7 @@
     <row r="1" spans="2:9" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="43"/>
@@ -4123,10 +4257,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -4156,214 +4290,214 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
     <row r="7" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
     </row>
     <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="148" t="s">
+      <c r="B9" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="148"/>
-      <c r="D9" s="149" t="s">
+      <c r="C9" s="121"/>
+      <c r="D9" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="149"/>
-      <c r="F9" s="149"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
       <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="148"/>
-      <c r="D10" s="150" t="s">
+      <c r="C10" s="121"/>
+      <c r="D10" s="122" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="123"/>
+      <c r="D11" s="124" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
+      <c r="H11" s="30"/>
+    </row>
+    <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="H12" s="30"/>
+    </row>
+    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="125" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="125"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="125"/>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="127" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="127"/>
+      <c r="E14" s="128" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="128"/>
+    </row>
+    <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="126"/>
+      <c r="C15" s="127"/>
+      <c r="D15" s="127"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="128"/>
+    </row>
+    <row r="16" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="50">
+        <v>1</v>
+      </c>
+      <c r="C16" s="139" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="139"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="140"/>
+    </row>
+    <row r="17" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="50">
+        <v>2</v>
+      </c>
+      <c r="C17" s="139" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="139"/>
+      <c r="E17" s="140"/>
+      <c r="F17" s="140"/>
+    </row>
+    <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="51">
+        <v>3</v>
+      </c>
+      <c r="C18" s="139" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="150"/>
-      <c r="F10" s="150"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="151" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="151"/>
-      <c r="D11" s="152" t="s">
+      <c r="D18" s="139"/>
+      <c r="E18" s="140"/>
+      <c r="F18" s="140"/>
+    </row>
+    <row r="19" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="51">
+        <v>4</v>
+      </c>
+      <c r="C19" s="139"/>
+      <c r="D19" s="139"/>
+      <c r="E19" s="140" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="152"/>
-      <c r="F11" s="152"/>
-      <c r="H11" s="30"/>
-    </row>
-    <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="153"/>
-      <c r="C12" s="154"/>
-      <c r="D12" s="154"/>
-      <c r="E12" s="154"/>
-      <c r="F12" s="154"/>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="155" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="155"/>
-      <c r="E13" s="155"/>
-      <c r="F13" s="155"/>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="156" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="157" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="157"/>
-      <c r="E14" s="158" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="158"/>
-    </row>
-    <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="156"/>
-      <c r="C15" s="157"/>
-      <c r="D15" s="157"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-    </row>
-    <row r="16" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="159">
-        <v>1</v>
-      </c>
-      <c r="C16" s="160" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="160"/>
-      <c r="E16" s="161"/>
-      <c r="F16" s="161"/>
-    </row>
-    <row r="17" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="159">
-        <v>2</v>
-      </c>
-      <c r="C17" s="160" t="s">
+      <c r="F19" s="140"/>
+    </row>
+    <row r="20" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="51">
+        <v>5</v>
+      </c>
+      <c r="C20" s="139" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="160"/>
-      <c r="E17" s="161"/>
-      <c r="F17" s="161"/>
-    </row>
-    <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="162">
-        <v>3</v>
-      </c>
-      <c r="C18" s="160" t="s">
+      <c r="D20" s="139"/>
+      <c r="E20" s="140"/>
+      <c r="F20" s="140"/>
+    </row>
+    <row r="21" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="51">
+        <v>6</v>
+      </c>
+      <c r="C21" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="160"/>
-      <c r="E18" s="161"/>
-      <c r="F18" s="161"/>
-    </row>
-    <row r="19" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="162">
-        <v>4</v>
-      </c>
-      <c r="C19" s="160"/>
-      <c r="D19" s="160"/>
-      <c r="E19" s="161" t="s">
+      <c r="D21" s="139"/>
+      <c r="E21" s="140"/>
+      <c r="F21" s="140"/>
+    </row>
+    <row r="22" spans="2:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="52">
+        <v>7</v>
+      </c>
+      <c r="C22" s="117"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="161"/>
-    </row>
-    <row r="20" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="162">
-        <v>5</v>
-      </c>
-      <c r="C20" s="160" t="s">
+      <c r="F22" s="118"/>
+    </row>
+    <row r="23" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+    </row>
+    <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+    </row>
+    <row r="25" spans="2:6" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="120" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="160"/>
-      <c r="E20" s="161"/>
-      <c r="F20" s="161"/>
-    </row>
-    <row r="21" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="162">
-        <v>6</v>
-      </c>
-      <c r="C21" s="160" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="160"/>
-      <c r="E21" s="161"/>
-      <c r="F21" s="161"/>
-    </row>
-    <row r="22" spans="2:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="163">
-        <v>7</v>
-      </c>
-      <c r="C22" s="164"/>
-      <c r="D22" s="164"/>
-      <c r="E22" s="165" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="165"/>
-    </row>
-    <row r="23" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="153"/>
-      <c r="C23" s="154"/>
-      <c r="D23" s="154"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-    </row>
-    <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="166" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="166"/>
-      <c r="D24" s="166"/>
-      <c r="E24" s="154"/>
-      <c r="F24" s="154"/>
-    </row>
-    <row r="25" spans="2:6" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="167" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" s="167"/>
-      <c r="D25" s="167"/>
-      <c r="E25" s="168"/>
-      <c r="F25" s="168"/>
+      <c r="C25" s="120"/>
+      <c r="D25" s="120"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
     </row>
     <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="29"/>
@@ -4402,7 +4536,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="C4:D4"/>
@@ -4419,21 +4568,6 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4442,7 +4576,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H35"/>
+  <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -4461,7 +4595,7 @@
     <row r="1" spans="2:8" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -4479,10 +4613,10 @@
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="117" t="s">
+      <c r="C4" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="95"/>
+      <c r="D4" s="136"/>
       <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
@@ -4510,68 +4644,68 @@
       <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="120" t="s">
+      <c r="E6" s="148" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="121"/>
+      <c r="F6" s="149"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="2:8" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="119"/>
-      <c r="D7" s="94" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="95"/>
-      <c r="F7" s="96"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="135" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="136"/>
+      <c r="F7" s="137"/>
       <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="92" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="119"/>
-      <c r="D8" s="94" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="95"/>
-      <c r="F8" s="96"/>
+      <c r="B8" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="147"/>
+      <c r="D8" s="135" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="136"/>
+      <c r="F8" s="137"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="93"/>
-      <c r="D9" s="94" t="s">
+      <c r="C9" s="134"/>
+      <c r="D9" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="95"/>
-      <c r="F9" s="96"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="137"/>
     </row>
     <row r="10" spans="2:8" s="20" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="98" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="99"/>
-      <c r="F10" s="100"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="101" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="102"/>
+      <c r="F10" s="103"/>
     </row>
     <row r="11" spans="2:8" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="103" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="104"/>
-      <c r="F11" s="105"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="106" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
     </row>
     <row r="12" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
@@ -4581,195 +4715,197 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="126" t="s">
+      <c r="B13" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="127"/>
-      <c r="D13" s="127"/>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
-      <c r="G13" s="127"/>
-      <c r="H13" s="128"/>
+      <c r="C13" s="155"/>
+      <c r="D13" s="155"/>
+      <c r="E13" s="155"/>
+      <c r="F13" s="155"/>
+      <c r="G13" s="155"/>
+      <c r="H13" s="156"/>
     </row>
     <row r="14" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="150" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="123"/>
-      <c r="E14" s="122" t="s">
+      <c r="D14" s="151"/>
+      <c r="E14" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="123"/>
-      <c r="G14" s="89" t="s">
+      <c r="F14" s="151"/>
+      <c r="G14" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="91"/>
+      <c r="H14" s="115"/>
     </row>
     <row r="15" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="88"/>
-      <c r="C15" s="124"/>
-      <c r="D15" s="125"/>
-      <c r="E15" s="124"/>
-      <c r="F15" s="125"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="91"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="152"/>
+      <c r="D15" s="153"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="153"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="115"/>
     </row>
     <row r="16" spans="2:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="14">
         <v>1</v>
       </c>
-      <c r="C16" s="117"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="117" t="s">
+      <c r="C16" s="144"/>
+      <c r="D16" s="146"/>
+      <c r="E16" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="118"/>
-      <c r="G16" s="117"/>
-      <c r="H16" s="129"/>
+      <c r="F16" s="146"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="145"/>
     </row>
     <row r="17" spans="2:8" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21">
         <v>2</v>
       </c>
-      <c r="C17" s="110" t="s">
+      <c r="C17" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="111"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="110"/>
-      <c r="H17" s="113"/>
+      <c r="D17" s="142"/>
+      <c r="E17" s="141"/>
+      <c r="F17" s="142"/>
+      <c r="G17" s="141"/>
+      <c r="H17" s="143"/>
     </row>
     <row r="18" spans="2:8" s="16" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="14">
         <v>3</v>
       </c>
-      <c r="C18" s="110"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="110" t="s">
+      <c r="C18" s="141"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="111"/>
-      <c r="G18" s="110"/>
-      <c r="H18" s="113"/>
+      <c r="F18" s="142"/>
+      <c r="G18" s="141"/>
+      <c r="H18" s="143"/>
     </row>
     <row r="19" spans="2:8" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="21">
         <v>4</v>
       </c>
-      <c r="C19" s="110"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="110" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="111"/>
-      <c r="G19" s="110"/>
-      <c r="H19" s="113"/>
+      <c r="C19" s="141"/>
+      <c r="D19" s="142"/>
+      <c r="E19" s="141" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="142"/>
+      <c r="G19" s="141"/>
+      <c r="H19" s="143"/>
     </row>
     <row r="20" spans="2:8" s="16" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="21">
         <v>5</v>
       </c>
-      <c r="C20" s="110"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="110" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="111"/>
-      <c r="G20" s="110"/>
-      <c r="H20" s="113"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="142"/>
+      <c r="E20" s="141" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="142"/>
+      <c r="G20" s="141"/>
+      <c r="H20" s="143"/>
     </row>
     <row r="21" spans="2:8" s="16" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="21"/>
-      <c r="C21" s="110"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="110" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="111"/>
-      <c r="G21" s="110"/>
-      <c r="H21" s="113"/>
-    </row>
-    <row r="22" spans="2:8" s="16" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="21">
+        <v>6</v>
+      </c>
+      <c r="C21" s="141"/>
+      <c r="D21" s="142"/>
+      <c r="E21" s="141" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="142"/>
+      <c r="G21" s="141"/>
+      <c r="H21" s="143"/>
+    </row>
+    <row r="22" spans="2:8" s="16" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="21">
-        <v>6</v>
-      </c>
-      <c r="C22" s="110"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="110" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="111"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="113"/>
+        <v>7</v>
+      </c>
+      <c r="C22" s="141"/>
+      <c r="D22" s="142"/>
+      <c r="E22" s="141" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="142"/>
+      <c r="G22" s="141"/>
+      <c r="H22" s="143"/>
     </row>
     <row r="23" spans="2:8" s="16" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="21">
-        <v>7</v>
-      </c>
-      <c r="C23" s="110"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="110" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="141"/>
+      <c r="D23" s="142"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="142"/>
+      <c r="G23" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="113"/>
+      <c r="H23" s="143"/>
     </row>
     <row r="24" spans="2:8" s="16" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="21">
-        <v>8</v>
-      </c>
-      <c r="C24" s="110"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="110" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="111"/>
-      <c r="G24" s="110"/>
-      <c r="H24" s="113"/>
+        <v>9</v>
+      </c>
+      <c r="C24" s="141"/>
+      <c r="D24" s="142"/>
+      <c r="E24" s="141" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="142"/>
+      <c r="G24" s="141"/>
+      <c r="H24" s="143"/>
     </row>
     <row r="25" spans="2:8" s="16" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="21">
-        <v>9</v>
-      </c>
-      <c r="C25" s="110"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="110" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="111"/>
-      <c r="G25" s="110"/>
-      <c r="H25" s="113"/>
+        <v>10</v>
+      </c>
+      <c r="C25" s="141"/>
+      <c r="D25" s="142"/>
+      <c r="E25" s="141" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="142"/>
+      <c r="G25" s="141"/>
+      <c r="H25" s="143"/>
     </row>
     <row r="26" spans="2:8" s="16" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="21">
-        <v>10</v>
-      </c>
-      <c r="C26" s="110"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="110" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="141"/>
+      <c r="D26" s="142"/>
+      <c r="E26" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="111"/>
-      <c r="G26" s="110"/>
-      <c r="H26" s="113"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="141"/>
+      <c r="H26" s="143"/>
     </row>
     <row r="27" spans="2:8" s="16" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15">
-        <v>11</v>
-      </c>
-      <c r="C27" s="114" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="157" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="115"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="115"/>
-      <c r="G27" s="114"/>
-      <c r="H27" s="116"/>
+      <c r="D27" s="158"/>
+      <c r="E27" s="157"/>
+      <c r="F27" s="158"/>
+      <c r="G27" s="157"/>
+      <c r="H27" s="159"/>
     </row>
     <row r="28" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
@@ -4779,52 +4915,56 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="2:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="112" t="s">
+      <c r="B29" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="85"/>
-      <c r="D29" s="86"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="95"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="107" t="s">
+      <c r="B30" s="160" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="108"/>
-      <c r="D30" s="109"/>
+      <c r="C30" s="161"/>
+      <c r="D30" s="162"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="2:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="107" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="108"/>
-      <c r="D31" s="109"/>
+    <row r="31" spans="2:8" s="16" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="160" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="161"/>
+      <c r="D31" s="162"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="2:8" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="106" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="104"/>
-      <c r="D32" s="105"/>
+    <row r="32" spans="2:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="160" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="161"/>
+      <c r="D32" s="162"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
+    <row r="33" spans="2:6" s="16" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="160" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="161"/>
+      <c r="D33" s="162"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
+    <row r="34" spans="2:6" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="96" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="97"/>
+      <c r="D34" s="98"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
@@ -4835,27 +4975,46 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
+    <row r="36" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C17:D17"/>
+  <mergeCells count="59">
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="B7:C7"/>
@@ -4872,28 +5031,25 @@
     <mergeCell ref="B13:H13"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="G14:H15"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4921,7 +5077,7 @@
     <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -4939,10 +5095,10 @@
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="117" t="s">
+      <c r="C4" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="95"/>
+      <c r="D4" s="136"/>
       <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
@@ -4970,68 +5126,68 @@
       <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="120" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="121"/>
+      <c r="E6" s="148" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="149"/>
       <c r="G6" s="17"/>
     </row>
     <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="119"/>
-      <c r="D7" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="95"/>
-      <c r="F7" s="96"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="135" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="136"/>
+      <c r="F7" s="137"/>
       <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="147"/>
+      <c r="D8" s="135" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="119"/>
-      <c r="D8" s="94" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="95"/>
-      <c r="F8" s="96"/>
+      <c r="E8" s="136"/>
+      <c r="F8" s="137"/>
       <c r="G8" s="17"/>
     </row>
     <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="131" t="s">
+      <c r="B9" s="171" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="131"/>
-      <c r="D9" s="132" t="s">
+      <c r="C9" s="171"/>
+      <c r="D9" s="172" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="132"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
     </row>
     <row r="10" spans="2:7" s="20" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="131" t="s">
+      <c r="B10" s="171" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="131"/>
-      <c r="D10" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="133"/>
-      <c r="F10" s="133"/>
+      <c r="C10" s="171"/>
+      <c r="D10" s="173" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="173"/>
+      <c r="F10" s="173"/>
     </row>
     <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="134" t="s">
+      <c r="B11" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="134"/>
-      <c r="D11" s="135" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
+      <c r="C11" s="174"/>
+      <c r="D11" s="175" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="175"/>
+      <c r="F11" s="175"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
@@ -5041,88 +5197,88 @@
       <c r="F12" s="23"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="136" t="s">
+      <c r="B13" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="136"/>
-      <c r="F13" s="136"/>
+      <c r="C13" s="176"/>
+      <c r="D13" s="176"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="176"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="137" t="s">
+      <c r="B14" s="177" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="138" t="s">
+      <c r="C14" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="138"/>
-      <c r="E14" s="122" t="s">
+      <c r="D14" s="167"/>
+      <c r="E14" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="139"/>
+      <c r="F14" s="168"/>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="137"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="124"/>
-      <c r="F15" s="140"/>
+      <c r="B15" s="177"/>
+      <c r="C15" s="167"/>
+      <c r="D15" s="167"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="169"/>
     </row>
     <row r="16" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="24">
         <v>1</v>
       </c>
-      <c r="C16" s="141"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="110" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="113"/>
+      <c r="C16" s="163"/>
+      <c r="D16" s="163"/>
+      <c r="E16" s="141" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="143"/>
     </row>
     <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="25">
         <v>2</v>
       </c>
-      <c r="C17" s="141" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="141"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="113"/>
+      <c r="C17" s="163" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="163"/>
+      <c r="E17" s="141"/>
+      <c r="F17" s="143"/>
     </row>
     <row r="18" spans="2:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="24">
         <v>3</v>
       </c>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="110" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="113"/>
+      <c r="C18" s="163"/>
+      <c r="D18" s="163"/>
+      <c r="E18" s="141" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="143"/>
     </row>
     <row r="19" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="25">
         <v>4</v>
       </c>
-      <c r="C19" s="141"/>
-      <c r="D19" s="141"/>
-      <c r="E19" s="110" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="113"/>
+      <c r="C19" s="163"/>
+      <c r="D19" s="163"/>
+      <c r="E19" s="141" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="143"/>
     </row>
     <row r="20" spans="2:6" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15">
         <v>5</v>
       </c>
-      <c r="C20" s="142"/>
-      <c r="D20" s="142"/>
-      <c r="E20" s="143" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="144"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="165" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="166"/>
     </row>
     <row r="21" spans="2:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="22"/>
@@ -5132,20 +5288,20 @@
       <c r="F21" s="23"/>
     </row>
     <row r="22" spans="2:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="130" t="s">
+      <c r="B22" s="170" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="130"/>
-      <c r="D22" s="130"/>
+      <c r="C22" s="170"/>
+      <c r="D22" s="170"/>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
     </row>
     <row r="23" spans="2:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="106" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="104"/>
-      <c r="D23" s="105"/>
+      <c r="B23" s="96" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="97"/>
+      <c r="D23" s="98"/>
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
     </row>
@@ -5172,18 +5328,6 @@
     <row r="32" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="C4:D4"/>
@@ -5200,6 +5344,18 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5210,7 +5366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5227,7 +5383,7 @@
     <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="45" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="43"/>
@@ -5245,10 +5401,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -5276,68 +5432,68 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
+      <c r="E6" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="57"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="72"/>
-      <c r="G6" s="30"/>
-    </row>
-    <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="G7" s="30"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="67" t="s">
+      <c r="C9" s="133"/>
+      <c r="D9" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="68"/>
-      <c r="F9" s="69"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="61"/>
     </row>
     <row r="10" spans="2:7" s="35" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="145" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="146"/>
-      <c r="F10" s="147"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="178" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="179"/>
+      <c r="F10" s="180"/>
     </row>
     <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="31"/>
@@ -5347,77 +5503,77 @@
       <c r="F12" s="30"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="52"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="79"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="59" t="s">
+      <c r="D14" s="83"/>
+      <c r="E14" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="61"/>
+      <c r="F14" s="84"/>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="58"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
     </row>
     <row r="16" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="34">
         <v>1</v>
       </c>
-      <c r="C16" s="62" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="64"/>
+      <c r="C16" s="85" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="86"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="91"/>
     </row>
     <row r="17" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="33">
         <v>2</v>
       </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="64"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="85" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="91"/>
     </row>
     <row r="18" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="33">
         <v>3</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" s="64"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="85" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="91"/>
     </row>
     <row r="19" spans="2:6" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="32">
         <v>4</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="49"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="89"/>
     </row>
     <row r="20" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="31"/>
@@ -5427,20 +5583,20 @@
       <c r="F20" s="30"/>
     </row>
     <row r="21" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="79"/>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
     <row r="22" spans="2:6" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
+      <c r="B22" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="74"/>
+      <c r="D22" s="75"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
     </row>
@@ -5488,6 +5644,24 @@
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="C17:D17"/>
@@ -5496,24 +5670,6 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Project final version :)
</commit_message>
<xml_diff>
--- a/Deliverables/RASD/Use Case specification 0.2.xlsx
+++ b/Deliverables/RASD/Use Case specification 0.2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="645" windowWidth="16590" windowHeight="8415"/>
+    <workbookView xWindow="4395" yWindow="645" windowWidth="16590" windowHeight="8415" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="UC-01" sheetId="18" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="114">
   <si>
     <t>No.</t>
   </si>
@@ -212,40 +212,11 @@
     <t>Informs the system that he accepts the request.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Sends the </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>incoming request information</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to the first available taxi driver in the zone's queue.</t>
-    </r>
-  </si>
-  <si>
     <t>Change the status of the taxi driver to not available.</t>
   </si>
   <si>
     <t>The taxi driver has accepted the request.
 The passenger is waiting for the system to reply to his request.</t>
-  </si>
-  <si>
-    <t>6.1. The zone's queue is empty or every taxi driver cancels the request:
-- The system informs the passenger(s) that it is impossible to find a taxi driver.
-- The Use Case ends.</t>
   </si>
   <si>
     <t>7.1. The taxi driver does not accept the request:
@@ -275,9 +246,6 @@
   </si>
   <si>
     <t>Confirms to the passenger that his cancel request has been taking to account.</t>
-  </si>
-  <si>
-    <t>Sends a message to the concerning taxi driver to inform him that the ride has been cancelled</t>
   </si>
   <si>
     <t>Puts the taxi driver at the top of the queue of the area he is related now</t>
@@ -685,9 +653,83 @@
     <t>Creates the passenger account in the MyTaxiService system.</t>
   </si>
   <si>
+    <t>3.1. The received information is not correct or complete:
+- The system informs the passeger that the sent information is wrong or incomplete.
+- Return to step 1.</t>
+  </si>
+  <si>
+    <t>The passenger is logged in MyTaxiService.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sends a form to the passengr with fields already filled corresponding to his personal information and two fields </t>
+  </si>
+  <si>
+    <t>6.1. The received information is not correct or complete:
+- The system informs the passeger that the sent information is wrong or incomplete.
+- Return to step 1.</t>
+  </si>
+  <si>
+    <t>Asks the passenger his email address and password.</t>
+  </si>
+  <si>
+    <t>Replies the system with his email address and password.</t>
+  </si>
+  <si>
+    <t>3.1 The passenger select: "Changes my password" :
+- The system send a three forms field, two for the same new password, one for the current one
+- The passeger fills the form
+- Return to the step 5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sends the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>incoming request information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to the first available taxi driver in the zone's queue whose capacity is greater or equal than the amount of people.</t>
+    </r>
+  </si>
+  <si>
+    <t>6.1. The zone queue is empty:
+- The system tries to find taxi drivers in the closest adjacent zones to the origins of the request (or the origin of thr first request for sharing requests)
+- Return to step 6.</t>
+  </si>
+  <si>
+    <t>Sends a message to the concerning taxi driver and passenger(s) to inform him that the ride has been cancelled</t>
+  </si>
+  <si>
+    <t>6.1. No accepting taxi driver is found within three minutes (neither in the one nor in the adjacent ones):
+- The system informs the passenger(s) that it is impossible to find a taxi driver.
+- The Use Case ends.</t>
+  </si>
+  <si>
+    <t>7.2. The taxi driver does not respond in less than 30 seconds:
+- The system sends the taxi driver to the bottom of the zone's queue.
+- Return to step 6.</t>
+  </si>
+  <si>
+    <t>Sends confirmation email to the passenger</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">The passenger is already registered in MyTaxiService.
-The taxi driver has not logged in MyTaxiService yet.
+The passeger has already confirmed his email address.
+The passenger has not logged in MyTaxiService yet.
 The passenger has launched the MyTaxiService mobile application or is the website.
 The passenger selects the option </t>
     </r>
@@ -710,17 +752,6 @@
       </rPr>
       <t>.</t>
     </r>
-  </si>
-  <si>
-    <t>3.1. The received information is not correct or complete:
-- The system informs the passeger that the sent information is wrong or incomplete.
-- Return to step 1.</t>
-  </si>
-  <si>
-    <t>3.1 The passenger select: "Changes my password" :
-- The system send a three forms field, two for the same new password, one for the current one
-- The taxi drivers fills the form
-- Return to the step 5</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1035,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1673,12 +1704,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF333399"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF333399"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF333399"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF333399"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF333399"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF333399"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF333399"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF333399"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF333399"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1797,29 +1867,88 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1836,76 +1965,136 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1914,35 +2103,69 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1953,63 +2176,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2035,27 +2221,6 @@
     <xf numFmtId="0" fontId="21" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2065,93 +2230,19 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2465,9 +2556,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I30"/>
+  <dimension ref="B1:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2502,10 +2593,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -2535,73 +2626,73 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
     <row r="7" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
     </row>
     <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="172" t="s">
+      <c r="B9" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="173"/>
-      <c r="D9" s="169" t="s">
+      <c r="C9" s="63"/>
+      <c r="D9" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="170"/>
-      <c r="F9" s="171"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66"/>
       <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:9" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="75" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75"/>
       <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2613,108 +2704,112 @@
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="52"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="79"/>
       <c r="H13" s="30"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="59" t="s">
+      <c r="C14" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="83"/>
+      <c r="E14" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="61"/>
+      <c r="F14" s="84"/>
     </row>
     <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="58"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
     </row>
     <row r="16" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="34">
         <v>1</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="70" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="175"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="87"/>
     </row>
     <row r="17" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="33">
         <v>2</v>
       </c>
-      <c r="C17" s="70" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="174"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="64"/>
+      <c r="C17" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="90"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="91"/>
     </row>
     <row r="18" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="33">
         <v>3</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="70" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="175"/>
-    </row>
-    <row r="19" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="32">
+      <c r="C18" s="85"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="87"/>
+    </row>
+    <row r="19" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="33">
         <v>4</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="49"/>
-    </row>
-    <row r="20" spans="2:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="31"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-    </row>
-    <row r="21" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
+      <c r="C19" s="181"/>
+      <c r="D19" s="182"/>
+      <c r="E19" s="183" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="184"/>
+    </row>
+    <row r="20" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="32">
+        <v>5</v>
+      </c>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="89"/>
+    </row>
+    <row r="21" spans="2:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="31"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
-    <row r="22" spans="2:6" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="53" t="s">
+    <row r="22" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="78"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+    </row>
+    <row r="23" spans="2:6" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-    </row>
-    <row r="23" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="75"/>
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
     </row>
@@ -2767,21 +2862,16 @@
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
     </row>
+    <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B22:D22"/>
+  <mergeCells count="28">
+    <mergeCell ref="B23:D23"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:D15"/>
@@ -2790,11 +2880,25 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B22:D22"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2803,7 +2907,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I28"/>
+  <dimension ref="B1:I29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -2840,10 +2944,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -2873,164 +2977,169 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
     <row r="7" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
     </row>
     <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
     </row>
-    <row r="9" spans="2:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="92" t="s">
+    <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="63"/>
+      <c r="D9" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66"/>
+      <c r="H9" s="30"/>
+    </row>
+    <row r="10" spans="2:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="97"/>
-      <c r="D9" s="98" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="99"/>
-      <c r="F9" s="100"/>
-      <c r="H9" s="30"/>
-    </row>
-    <row r="10" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="101" t="s">
+      <c r="C10" s="100"/>
+      <c r="D10" s="101" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="102"/>
+      <c r="F10" s="103"/>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="103" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="104"/>
-      <c r="F10" s="105"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="106" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
       <c r="H11" s="30"/>
     </row>
-    <row r="12" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="84" t="s">
+    <row r="12" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="H12" s="30"/>
+    </row>
+    <row r="13" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85"/>
-      <c r="F12" s="86"/>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="87" t="s">
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="95"/>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="89" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="90"/>
-      <c r="E13" s="89" t="s">
+      <c r="C14" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="114"/>
+      <c r="E14" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="91"/>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="88"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="91"/>
-    </row>
-    <row r="15" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="14">
+      <c r="F14" s="115"/>
+      <c r="H14" s="30"/>
+    </row>
+    <row r="15" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="112"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="115"/>
+    </row>
+    <row r="16" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="14">
         <v>1</v>
       </c>
-      <c r="C15" s="81"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="81" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="83"/>
-    </row>
-    <row r="16" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="21">
+      <c r="C16" s="107"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="107" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" s="109"/>
+    </row>
+    <row r="17" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="21">
         <v>2</v>
       </c>
-      <c r="C16" s="81" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="82"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="83"/>
-    </row>
-    <row r="17" spans="2:6" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="32">
+      <c r="C17" s="107" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="108"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="109"/>
+    </row>
+    <row r="18" spans="2:6" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="32">
         <v>3</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="49"/>
-    </row>
-    <row r="18" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="31"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-    </row>
-    <row r="19" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="112" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="85"/>
-      <c r="D19" s="86"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="89"/>
+    </row>
+    <row r="19" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="31"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
     </row>
-    <row r="20" spans="2:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="106" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="104"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-    </row>
-    <row r="21" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
+    <row r="20" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="94"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="2:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="96" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="97"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
     </row>
@@ -3083,30 +3192,39 @@
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
     </row>
+    <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+    </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
+  <mergeCells count="24">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3115,7 +3233,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I30"/>
+  <dimension ref="B1:I31"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3134,7 +3252,7 @@
     <row r="1" spans="2:9" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="45" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="43"/>
@@ -3152,10 +3270,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -3185,226 +3303,232 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
     <row r="7" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
     </row>
     <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="172" t="s">
+      <c r="B9" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="173"/>
-      <c r="D9" s="169" t="s">
+      <c r="C9" s="63"/>
+      <c r="D9" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="170"/>
-      <c r="F9" s="171"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66"/>
       <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="148"/>
-      <c r="D10" s="150" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="150"/>
-      <c r="F10" s="150"/>
+      <c r="C10" s="121"/>
+      <c r="D10" s="122" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="151" t="s">
+      <c r="B11" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="151"/>
-      <c r="D11" s="152" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="152"/>
-      <c r="F11" s="152"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="124" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
       <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="153"/>
-      <c r="C12" s="154"/>
-      <c r="D12" s="154"/>
-      <c r="E12" s="154"/>
-      <c r="F12" s="154"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="155"/>
-      <c r="E13" s="155"/>
-      <c r="F13" s="155"/>
+      <c r="C13" s="125"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="125"/>
       <c r="H13" s="30"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="157" t="s">
+      <c r="C14" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="157"/>
-      <c r="E14" s="158" t="s">
+      <c r="D14" s="127"/>
+      <c r="E14" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="158"/>
+      <c r="F14" s="128"/>
     </row>
     <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="156"/>
-      <c r="C15" s="157"/>
-      <c r="D15" s="157"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="127"/>
+      <c r="D15" s="127"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="128"/>
     </row>
     <row r="16" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="159">
+      <c r="B16" s="50">
         <v>1</v>
       </c>
-      <c r="C16" s="177" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16" s="177"/>
-      <c r="E16" s="178"/>
-      <c r="F16" s="178"/>
+      <c r="C16" s="129" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="129"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="130"/>
     </row>
     <row r="17" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="159">
+      <c r="B17" s="50">
         <v>2</v>
       </c>
-      <c r="C17" s="177" t="s">
+      <c r="C17" s="129" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="129"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="130"/>
+    </row>
+    <row r="18" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="51">
+        <v>3</v>
+      </c>
+      <c r="C18" s="129" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="129"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="130"/>
+    </row>
+    <row r="19" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="51">
+        <v>4</v>
+      </c>
+      <c r="C19" s="129"/>
+      <c r="D19" s="129"/>
+      <c r="E19" s="130" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="130"/>
+    </row>
+    <row r="20" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="51">
+        <v>5</v>
+      </c>
+      <c r="C20" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="177"/>
-      <c r="E17" s="178"/>
-      <c r="F17" s="178"/>
-    </row>
-    <row r="18" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="162">
-        <v>3</v>
-      </c>
-      <c r="C18" s="177" t="s">
+      <c r="D20" s="129"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="130"/>
+    </row>
+    <row r="21" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="51">
+        <v>6</v>
+      </c>
+      <c r="C21" s="129"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="131" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="177"/>
-      <c r="E18" s="178"/>
-      <c r="F18" s="178"/>
-    </row>
-    <row r="19" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="162">
-        <v>4</v>
-      </c>
-      <c r="C19" s="177"/>
-      <c r="D19" s="177"/>
-      <c r="E19" s="178" t="s">
+      <c r="F21" s="132"/>
+    </row>
+    <row r="22" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="51">
+        <v>7</v>
+      </c>
+      <c r="C22" s="131"/>
+      <c r="D22" s="185"/>
+      <c r="E22" s="183" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="184"/>
+    </row>
+    <row r="23" spans="2:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="52">
+        <v>8</v>
+      </c>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="178"/>
-    </row>
-    <row r="20" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="162">
-        <v>5</v>
-      </c>
-      <c r="C20" s="177" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="177"/>
-      <c r="E20" s="178"/>
-      <c r="F20" s="178"/>
-    </row>
-    <row r="21" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="162">
-        <v>6</v>
-      </c>
-      <c r="C21" s="177" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="177"/>
-      <c r="E21" s="178"/>
-      <c r="F21" s="178"/>
-    </row>
-    <row r="22" spans="2:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="163">
-        <v>7</v>
-      </c>
-      <c r="C22" s="164"/>
-      <c r="D22" s="164"/>
-      <c r="E22" s="165" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="165"/>
-    </row>
-    <row r="23" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="153"/>
-      <c r="C23" s="154"/>
-      <c r="D23" s="154"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-    </row>
-    <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="166" t="s">
+      <c r="F23" s="118"/>
+    </row>
+    <row r="24" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="48"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+    </row>
+    <row r="25" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="166"/>
-      <c r="D24" s="166"/>
-      <c r="E24" s="154"/>
-      <c r="F24" s="154"/>
-    </row>
-    <row r="25" spans="2:6" ht="78" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="176" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" s="167"/>
-      <c r="D25" s="167"/>
-      <c r="E25" s="168"/>
-      <c r="F25" s="168"/>
-    </row>
-    <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-    </row>
-    <row r="27" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+    </row>
+    <row r="26" spans="2:6" ht="78" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="119" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="120"/>
+      <c r="D26" s="120"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+    </row>
+    <row r="27" spans="2:6" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="96" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="97"/>
+      <c r="D27" s="98"/>
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
     </row>
@@ -3429,40 +3553,50 @@
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
     </row>
+    <row r="31" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+    </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="B24:D24"/>
+  <mergeCells count="35">
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3490,7 +3624,7 @@
     <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="43"/>
@@ -3508,10 +3642,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -3539,68 +3673,68 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="G6" s="30"/>
     </row>
     <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="G7" s="30"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="67" t="s">
+      <c r="C9" s="133"/>
+      <c r="D9" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="68"/>
-      <c r="F9" s="69"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="61"/>
     </row>
     <row r="10" spans="2:7" s="35" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="75" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="76"/>
-      <c r="F10" s="77"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
     </row>
     <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="31"/>
@@ -3610,77 +3744,77 @@
       <c r="F12" s="30"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="52"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="79"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="59" t="s">
+      <c r="D14" s="83"/>
+      <c r="E14" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="61"/>
+      <c r="F14" s="84"/>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="58"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
     </row>
     <row r="16" spans="2:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="34">
         <v>1</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="64"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="85" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="91"/>
     </row>
     <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="33">
         <v>2</v>
       </c>
-      <c r="C17" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="64"/>
+      <c r="C17" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="86"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="91"/>
     </row>
     <row r="18" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="33">
         <v>3</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="64"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="91"/>
     </row>
     <row r="19" spans="2:6" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="32">
         <v>4</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="49"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="89"/>
     </row>
     <row r="20" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="31"/>
@@ -3690,20 +3824,20 @@
       <c r="F20" s="30"/>
     </row>
     <row r="21" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="79"/>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
     <row r="22" spans="2:6" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
+      <c r="B22" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="74"/>
+      <c r="D22" s="75"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
     </row>
@@ -3751,6 +3885,18 @@
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B13:F13"/>
@@ -3765,18 +3911,6 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3804,7 +3938,7 @@
     <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="45" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="43"/>
@@ -3822,10 +3956,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -3853,68 +3987,68 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="G6" s="30"/>
     </row>
     <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="G7" s="30"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="93"/>
-      <c r="D9" s="94" t="s">
+      <c r="C9" s="134"/>
+      <c r="D9" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="95"/>
-      <c r="F9" s="96"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="137"/>
     </row>
     <row r="10" spans="2:7" s="35" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="98" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="99"/>
-      <c r="F10" s="100"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="102"/>
+      <c r="F10" s="103"/>
     </row>
     <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="103" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="104"/>
-      <c r="F11" s="105"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="106" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
@@ -3924,66 +4058,66 @@
       <c r="F12" s="17"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="86"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="95"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="90"/>
-      <c r="E14" s="89" t="s">
+      <c r="D14" s="114"/>
+      <c r="E14" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="91"/>
+      <c r="F14" s="115"/>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="88"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="91"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="115"/>
     </row>
     <row r="16" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="14">
         <v>1</v>
       </c>
-      <c r="C16" s="81"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="81" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="83"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="107" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="109"/>
     </row>
     <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21">
         <v>2</v>
       </c>
-      <c r="C17" s="81" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="82"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="83"/>
+      <c r="C17" s="107" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="108"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="109"/>
     </row>
     <row r="18" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="32">
         <v>3</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="49"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="89"/>
     </row>
     <row r="19" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="31"/>
@@ -3993,20 +4127,20 @@
       <c r="F19" s="30"/>
     </row>
     <row r="20" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="112" t="s">
+      <c r="B20" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="85"/>
-      <c r="D20" s="86"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="95"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
     </row>
     <row r="21" spans="2:6" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="106" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="104"/>
-      <c r="D21" s="105"/>
+      <c r="B21" s="96" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="97"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
     </row>
@@ -4054,18 +4188,6 @@
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="C17:D17"/>
@@ -4078,6 +4200,18 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4105,7 +4239,7 @@
     <row r="1" spans="2:9" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="43"/>
@@ -4123,10 +4257,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -4156,214 +4290,214 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="72"/>
+      <c r="E6" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
     <row r="7" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
     </row>
     <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="148" t="s">
+      <c r="B9" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="148"/>
-      <c r="D9" s="149" t="s">
+      <c r="C9" s="121"/>
+      <c r="D9" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="149"/>
-      <c r="F9" s="149"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
       <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="148"/>
-      <c r="D10" s="150" t="s">
+      <c r="C10" s="121"/>
+      <c r="D10" s="122" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="123"/>
+      <c r="D11" s="124" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
+      <c r="H11" s="30"/>
+    </row>
+    <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="H12" s="30"/>
+    </row>
+    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="125" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="125"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="125"/>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="127" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="127"/>
+      <c r="E14" s="128" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="128"/>
+    </row>
+    <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="126"/>
+      <c r="C15" s="127"/>
+      <c r="D15" s="127"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="128"/>
+    </row>
+    <row r="16" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="50">
+        <v>1</v>
+      </c>
+      <c r="C16" s="139" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="139"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="140"/>
+    </row>
+    <row r="17" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="50">
+        <v>2</v>
+      </c>
+      <c r="C17" s="139" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="139"/>
+      <c r="E17" s="140"/>
+      <c r="F17" s="140"/>
+    </row>
+    <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="51">
+        <v>3</v>
+      </c>
+      <c r="C18" s="139" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="150"/>
-      <c r="F10" s="150"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="151" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="151"/>
-      <c r="D11" s="152" t="s">
+      <c r="D18" s="139"/>
+      <c r="E18" s="140"/>
+      <c r="F18" s="140"/>
+    </row>
+    <row r="19" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="51">
+        <v>4</v>
+      </c>
+      <c r="C19" s="139"/>
+      <c r="D19" s="139"/>
+      <c r="E19" s="140" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="152"/>
-      <c r="F11" s="152"/>
-      <c r="H11" s="30"/>
-    </row>
-    <row r="12" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="153"/>
-      <c r="C12" s="154"/>
-      <c r="D12" s="154"/>
-      <c r="E12" s="154"/>
-      <c r="F12" s="154"/>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="155" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="155"/>
-      <c r="E13" s="155"/>
-      <c r="F13" s="155"/>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="156" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="157" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="157"/>
-      <c r="E14" s="158" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="158"/>
-    </row>
-    <row r="15" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="156"/>
-      <c r="C15" s="157"/>
-      <c r="D15" s="157"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-    </row>
-    <row r="16" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="159">
-        <v>1</v>
-      </c>
-      <c r="C16" s="160" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="160"/>
-      <c r="E16" s="161"/>
-      <c r="F16" s="161"/>
-    </row>
-    <row r="17" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="159">
-        <v>2</v>
-      </c>
-      <c r="C17" s="160" t="s">
+      <c r="F19" s="140"/>
+    </row>
+    <row r="20" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="51">
+        <v>5</v>
+      </c>
+      <c r="C20" s="139" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="160"/>
-      <c r="E17" s="161"/>
-      <c r="F17" s="161"/>
-    </row>
-    <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="162">
-        <v>3</v>
-      </c>
-      <c r="C18" s="160" t="s">
+      <c r="D20" s="139"/>
+      <c r="E20" s="140"/>
+      <c r="F20" s="140"/>
+    </row>
+    <row r="21" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="51">
+        <v>6</v>
+      </c>
+      <c r="C21" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="160"/>
-      <c r="E18" s="161"/>
-      <c r="F18" s="161"/>
-    </row>
-    <row r="19" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="162">
-        <v>4</v>
-      </c>
-      <c r="C19" s="160"/>
-      <c r="D19" s="160"/>
-      <c r="E19" s="161" t="s">
+      <c r="D21" s="139"/>
+      <c r="E21" s="140"/>
+      <c r="F21" s="140"/>
+    </row>
+    <row r="22" spans="2:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="52">
+        <v>7</v>
+      </c>
+      <c r="C22" s="117"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="161"/>
-    </row>
-    <row r="20" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="162">
-        <v>5</v>
-      </c>
-      <c r="C20" s="160" t="s">
+      <c r="F22" s="118"/>
+    </row>
+    <row r="23" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+    </row>
+    <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+    </row>
+    <row r="25" spans="2:6" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="120" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="160"/>
-      <c r="E20" s="161"/>
-      <c r="F20" s="161"/>
-    </row>
-    <row r="21" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="162">
-        <v>6</v>
-      </c>
-      <c r="C21" s="160" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="160"/>
-      <c r="E21" s="161"/>
-      <c r="F21" s="161"/>
-    </row>
-    <row r="22" spans="2:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="163">
-        <v>7</v>
-      </c>
-      <c r="C22" s="164"/>
-      <c r="D22" s="164"/>
-      <c r="E22" s="165" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="165"/>
-    </row>
-    <row r="23" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="153"/>
-      <c r="C23" s="154"/>
-      <c r="D23" s="154"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-    </row>
-    <row r="24" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="166" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="166"/>
-      <c r="D24" s="166"/>
-      <c r="E24" s="154"/>
-      <c r="F24" s="154"/>
-    </row>
-    <row r="25" spans="2:6" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="167" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" s="167"/>
-      <c r="D25" s="167"/>
-      <c r="E25" s="168"/>
-      <c r="F25" s="168"/>
+      <c r="C25" s="120"/>
+      <c r="D25" s="120"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
     </row>
     <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="29"/>
@@ -4402,7 +4536,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="C4:D4"/>
@@ -4419,21 +4568,6 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4442,7 +4576,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H35"/>
+  <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -4461,7 +4595,7 @@
     <row r="1" spans="2:8" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -4479,10 +4613,10 @@
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="117" t="s">
+      <c r="C4" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="95"/>
+      <c r="D4" s="136"/>
       <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
@@ -4510,68 +4644,68 @@
       <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="120" t="s">
+      <c r="E6" s="148" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="121"/>
+      <c r="F6" s="149"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="2:8" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="119"/>
-      <c r="D7" s="94" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="95"/>
-      <c r="F7" s="96"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="135" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="136"/>
+      <c r="F7" s="137"/>
       <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="92" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="119"/>
-      <c r="D8" s="94" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="95"/>
-      <c r="F8" s="96"/>
+      <c r="B8" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="147"/>
+      <c r="D8" s="135" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="136"/>
+      <c r="F8" s="137"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="93"/>
-      <c r="D9" s="94" t="s">
+      <c r="C9" s="134"/>
+      <c r="D9" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="95"/>
-      <c r="F9" s="96"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="137"/>
     </row>
     <row r="10" spans="2:8" s="20" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="98" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="99"/>
-      <c r="F10" s="100"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="101" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="102"/>
+      <c r="F10" s="103"/>
     </row>
     <row r="11" spans="2:8" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="103" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="104"/>
-      <c r="F11" s="105"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="106" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
     </row>
     <row r="12" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
@@ -4581,195 +4715,197 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="126" t="s">
+      <c r="B13" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="127"/>
-      <c r="D13" s="127"/>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
-      <c r="G13" s="127"/>
-      <c r="H13" s="128"/>
+      <c r="C13" s="155"/>
+      <c r="D13" s="155"/>
+      <c r="E13" s="155"/>
+      <c r="F13" s="155"/>
+      <c r="G13" s="155"/>
+      <c r="H13" s="156"/>
     </row>
     <row r="14" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="150" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="123"/>
-      <c r="E14" s="122" t="s">
+      <c r="D14" s="151"/>
+      <c r="E14" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="123"/>
-      <c r="G14" s="89" t="s">
+      <c r="F14" s="151"/>
+      <c r="G14" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="91"/>
+      <c r="H14" s="115"/>
     </row>
     <row r="15" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="88"/>
-      <c r="C15" s="124"/>
-      <c r="D15" s="125"/>
-      <c r="E15" s="124"/>
-      <c r="F15" s="125"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="91"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="152"/>
+      <c r="D15" s="153"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="153"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="115"/>
     </row>
     <row r="16" spans="2:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="14">
         <v>1</v>
       </c>
-      <c r="C16" s="117"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="117" t="s">
+      <c r="C16" s="144"/>
+      <c r="D16" s="146"/>
+      <c r="E16" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="118"/>
-      <c r="G16" s="117"/>
-      <c r="H16" s="129"/>
+      <c r="F16" s="146"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="145"/>
     </row>
     <row r="17" spans="2:8" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21">
         <v>2</v>
       </c>
-      <c r="C17" s="110" t="s">
+      <c r="C17" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="111"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="110"/>
-      <c r="H17" s="113"/>
+      <c r="D17" s="142"/>
+      <c r="E17" s="141"/>
+      <c r="F17" s="142"/>
+      <c r="G17" s="141"/>
+      <c r="H17" s="143"/>
     </row>
     <row r="18" spans="2:8" s="16" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="14">
         <v>3</v>
       </c>
-      <c r="C18" s="110"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="110" t="s">
+      <c r="C18" s="141"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="111"/>
-      <c r="G18" s="110"/>
-      <c r="H18" s="113"/>
+      <c r="F18" s="142"/>
+      <c r="G18" s="141"/>
+      <c r="H18" s="143"/>
     </row>
     <row r="19" spans="2:8" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="21">
         <v>4</v>
       </c>
-      <c r="C19" s="110"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="110" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="111"/>
-      <c r="G19" s="110"/>
-      <c r="H19" s="113"/>
+      <c r="C19" s="141"/>
+      <c r="D19" s="142"/>
+      <c r="E19" s="141" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="142"/>
+      <c r="G19" s="141"/>
+      <c r="H19" s="143"/>
     </row>
     <row r="20" spans="2:8" s="16" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="21">
         <v>5</v>
       </c>
-      <c r="C20" s="110"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="110" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="111"/>
-      <c r="G20" s="110"/>
-      <c r="H20" s="113"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="142"/>
+      <c r="E20" s="141" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="142"/>
+      <c r="G20" s="141"/>
+      <c r="H20" s="143"/>
     </row>
     <row r="21" spans="2:8" s="16" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="21"/>
-      <c r="C21" s="110"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="110" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="111"/>
-      <c r="G21" s="110"/>
-      <c r="H21" s="113"/>
-    </row>
-    <row r="22" spans="2:8" s="16" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="21">
+        <v>6</v>
+      </c>
+      <c r="C21" s="141"/>
+      <c r="D21" s="142"/>
+      <c r="E21" s="141" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="142"/>
+      <c r="G21" s="141"/>
+      <c r="H21" s="143"/>
+    </row>
+    <row r="22" spans="2:8" s="16" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="21">
-        <v>6</v>
-      </c>
-      <c r="C22" s="110"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="110" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="111"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="113"/>
+        <v>7</v>
+      </c>
+      <c r="C22" s="141"/>
+      <c r="D22" s="142"/>
+      <c r="E22" s="141" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="142"/>
+      <c r="G22" s="141"/>
+      <c r="H22" s="143"/>
     </row>
     <row r="23" spans="2:8" s="16" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="21">
-        <v>7</v>
-      </c>
-      <c r="C23" s="110"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="110" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="141"/>
+      <c r="D23" s="142"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="142"/>
+      <c r="G23" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="113"/>
+      <c r="H23" s="143"/>
     </row>
     <row r="24" spans="2:8" s="16" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="21">
-        <v>8</v>
-      </c>
-      <c r="C24" s="110"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="110" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="111"/>
-      <c r="G24" s="110"/>
-      <c r="H24" s="113"/>
+        <v>9</v>
+      </c>
+      <c r="C24" s="141"/>
+      <c r="D24" s="142"/>
+      <c r="E24" s="141" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="142"/>
+      <c r="G24" s="141"/>
+      <c r="H24" s="143"/>
     </row>
     <row r="25" spans="2:8" s="16" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="21">
-        <v>9</v>
-      </c>
-      <c r="C25" s="110"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="110" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="111"/>
-      <c r="G25" s="110"/>
-      <c r="H25" s="113"/>
+        <v>10</v>
+      </c>
+      <c r="C25" s="141"/>
+      <c r="D25" s="142"/>
+      <c r="E25" s="141" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="142"/>
+      <c r="G25" s="141"/>
+      <c r="H25" s="143"/>
     </row>
     <row r="26" spans="2:8" s="16" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="21">
-        <v>10</v>
-      </c>
-      <c r="C26" s="110"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="110" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="141"/>
+      <c r="D26" s="142"/>
+      <c r="E26" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="111"/>
-      <c r="G26" s="110"/>
-      <c r="H26" s="113"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="141"/>
+      <c r="H26" s="143"/>
     </row>
     <row r="27" spans="2:8" s="16" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15">
-        <v>11</v>
-      </c>
-      <c r="C27" s="114" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="157" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="115"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="115"/>
-      <c r="G27" s="114"/>
-      <c r="H27" s="116"/>
+      <c r="D27" s="158"/>
+      <c r="E27" s="157"/>
+      <c r="F27" s="158"/>
+      <c r="G27" s="157"/>
+      <c r="H27" s="159"/>
     </row>
     <row r="28" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
@@ -4779,52 +4915,56 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="2:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="112" t="s">
+      <c r="B29" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="85"/>
-      <c r="D29" s="86"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="95"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="107" t="s">
+      <c r="B30" s="160" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="108"/>
-      <c r="D30" s="109"/>
+      <c r="C30" s="161"/>
+      <c r="D30" s="162"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="2:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="107" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="108"/>
-      <c r="D31" s="109"/>
+    <row r="31" spans="2:8" s="16" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="160" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="161"/>
+      <c r="D31" s="162"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="2:8" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="106" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="104"/>
-      <c r="D32" s="105"/>
+    <row r="32" spans="2:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="160" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="161"/>
+      <c r="D32" s="162"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
+    <row r="33" spans="2:6" s="16" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="160" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="161"/>
+      <c r="D33" s="162"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
+    <row r="34" spans="2:6" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="96" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="97"/>
+      <c r="D34" s="98"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
@@ -4835,27 +4975,46 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
+    <row r="36" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C17:D17"/>
+  <mergeCells count="59">
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="B7:C7"/>
@@ -4872,28 +5031,25 @@
     <mergeCell ref="B13:H13"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="G14:H15"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4921,7 +5077,7 @@
     <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -4939,10 +5095,10 @@
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="117" t="s">
+      <c r="C4" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="95"/>
+      <c r="D4" s="136"/>
       <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
@@ -4970,68 +5126,68 @@
       <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="120" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="121"/>
+      <c r="E6" s="148" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="149"/>
       <c r="G6" s="17"/>
     </row>
     <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="119"/>
-      <c r="D7" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="95"/>
-      <c r="F7" s="96"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="135" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="136"/>
+      <c r="F7" s="137"/>
       <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="147"/>
+      <c r="D8" s="135" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="119"/>
-      <c r="D8" s="94" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="95"/>
-      <c r="F8" s="96"/>
+      <c r="E8" s="136"/>
+      <c r="F8" s="137"/>
       <c r="G8" s="17"/>
     </row>
     <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="131" t="s">
+      <c r="B9" s="171" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="131"/>
-      <c r="D9" s="132" t="s">
+      <c r="C9" s="171"/>
+      <c r="D9" s="172" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="132"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
     </row>
     <row r="10" spans="2:7" s="20" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="131" t="s">
+      <c r="B10" s="171" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="131"/>
-      <c r="D10" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="133"/>
-      <c r="F10" s="133"/>
+      <c r="C10" s="171"/>
+      <c r="D10" s="173" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="173"/>
+      <c r="F10" s="173"/>
     </row>
     <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="134" t="s">
+      <c r="B11" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="134"/>
-      <c r="D11" s="135" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
+      <c r="C11" s="174"/>
+      <c r="D11" s="175" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="175"/>
+      <c r="F11" s="175"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
@@ -5041,88 +5197,88 @@
       <c r="F12" s="23"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="136" t="s">
+      <c r="B13" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="136"/>
-      <c r="F13" s="136"/>
+      <c r="C13" s="176"/>
+      <c r="D13" s="176"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="176"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="137" t="s">
+      <c r="B14" s="177" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="138" t="s">
+      <c r="C14" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="138"/>
-      <c r="E14" s="122" t="s">
+      <c r="D14" s="167"/>
+      <c r="E14" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="139"/>
+      <c r="F14" s="168"/>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="137"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="124"/>
-      <c r="F15" s="140"/>
+      <c r="B15" s="177"/>
+      <c r="C15" s="167"/>
+      <c r="D15" s="167"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="169"/>
     </row>
     <row r="16" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="24">
         <v>1</v>
       </c>
-      <c r="C16" s="141"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="110" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="113"/>
+      <c r="C16" s="163"/>
+      <c r="D16" s="163"/>
+      <c r="E16" s="141" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="143"/>
     </row>
     <row r="17" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="25">
         <v>2</v>
       </c>
-      <c r="C17" s="141" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="141"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="113"/>
+      <c r="C17" s="163" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="163"/>
+      <c r="E17" s="141"/>
+      <c r="F17" s="143"/>
     </row>
     <row r="18" spans="2:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="24">
         <v>3</v>
       </c>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="110" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="113"/>
+      <c r="C18" s="163"/>
+      <c r="D18" s="163"/>
+      <c r="E18" s="141" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="143"/>
     </row>
     <row r="19" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="25">
         <v>4</v>
       </c>
-      <c r="C19" s="141"/>
-      <c r="D19" s="141"/>
-      <c r="E19" s="110" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="113"/>
+      <c r="C19" s="163"/>
+      <c r="D19" s="163"/>
+      <c r="E19" s="141" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="143"/>
     </row>
     <row r="20" spans="2:6" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15">
         <v>5</v>
       </c>
-      <c r="C20" s="142"/>
-      <c r="D20" s="142"/>
-      <c r="E20" s="143" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="144"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="165" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="166"/>
     </row>
     <row r="21" spans="2:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="22"/>
@@ -5132,20 +5288,20 @@
       <c r="F21" s="23"/>
     </row>
     <row r="22" spans="2:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="130" t="s">
+      <c r="B22" s="170" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="130"/>
-      <c r="D22" s="130"/>
+      <c r="C22" s="170"/>
+      <c r="D22" s="170"/>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
     </row>
     <row r="23" spans="2:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="106" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="104"/>
-      <c r="D23" s="105"/>
+      <c r="B23" s="96" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="97"/>
+      <c r="D23" s="98"/>
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
     </row>
@@ -5172,18 +5328,6 @@
     <row r="32" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="C4:D4"/>
@@ -5200,6 +5344,18 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5210,7 +5366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5227,7 +5383,7 @@
     <row r="1" spans="2:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="45" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="43"/>
@@ -5245,10 +5401,10 @@
       <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
@@ -5276,68 +5432,68 @@
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="71" t="s">
+      <c r="E6" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="57"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="72"/>
-      <c r="G6" s="30"/>
-    </row>
-    <row r="7" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="65" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="61"/>
       <c r="G7" s="30"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="B8" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="67" t="s">
+      <c r="C9" s="133"/>
+      <c r="D9" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="68"/>
-      <c r="F9" s="69"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="61"/>
     </row>
     <row r="10" spans="2:7" s="35" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="145" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="146"/>
-      <c r="F10" s="147"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="178" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="179"/>
+      <c r="F10" s="180"/>
     </row>
     <row r="11" spans="2:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75"/>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="31"/>
@@ -5347,77 +5503,77 @@
       <c r="F12" s="30"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="52"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="79"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="59" t="s">
+      <c r="D14" s="83"/>
+      <c r="E14" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="61"/>
+      <c r="F14" s="84"/>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="58"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
     </row>
     <row r="16" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="34">
         <v>1</v>
       </c>
-      <c r="C16" s="62" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="64"/>
+      <c r="C16" s="85" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="86"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="91"/>
     </row>
     <row r="17" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="33">
         <v>2</v>
       </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="64"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="85" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="91"/>
     </row>
     <row r="18" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="33">
         <v>3</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" s="64"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="85" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="91"/>
     </row>
     <row r="19" spans="2:6" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="32">
         <v>4</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="49"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="89"/>
     </row>
     <row r="20" spans="2:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="31"/>
@@ -5427,20 +5583,20 @@
       <c r="F20" s="30"/>
     </row>
     <row r="21" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="79"/>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
     <row r="22" spans="2:6" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
+      <c r="B22" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="74"/>
+      <c r="D22" s="75"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
     </row>
@@ -5488,6 +5644,24 @@
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="C17:D17"/>
@@ -5496,24 +5670,6 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>